<commit_message>
memberType and user/companies import done
</commit_message>
<xml_diff>
--- a/frontend/src/assets/data/QuotaExample.xlsx
+++ b/frontend/src/assets/data/QuotaExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projeto\surf-management-app\frontend\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7381984C-FBD5-41FB-ADBB-4B3E2BEFC0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F86BC74-8547-4E57-BA7A-67877883FDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE2EA506-E2F7-4CC2-89E1-9B0543CB6F16}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
-  <si>
-    <t>email do membro</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>valor em euros</t>
   </si>
@@ -52,20 +49,14 @@
     <t>23/2/2021</t>
   </si>
   <si>
-    <t>joselopes@gmail.com</t>
-  </si>
-  <si>
-    <t>ripcurl@gmail.com</t>
-  </si>
-  <si>
-    <t>carlosafonso@gmail.com</t>
+    <t>Id do membro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,14 +67,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,10 +115,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -145,19 +127,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -473,7 +454,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,113 +467,106 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
+      <c r="A2" s="5">
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>15</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>44197</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
+      <c r="A3" s="5">
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>15</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>43831</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>43954</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
+      <c r="A4" s="5">
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>15</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>44197</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
+      <c r="A5" s="5">
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>43831</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>43958</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
+      <c r="A6" s="5">
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>50</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>44197</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>44410</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
+      <c r="A7" s="5">
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>50</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>44562</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{65C27F34-2FC2-4B98-9374-04AC5B2F0539}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{EF80D5D1-94E2-4E92-ACFB-F2AD856F5FB0}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{846DF2F1-FFAF-4145-AA8F-01C439D8473C}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{0DE545F7-73E0-435B-82C9-65A264DD67F1}"/>
-    <hyperlink ref="A6:A7" r:id="rId5" display="ripcurl@gmail.com" xr:uid="{ED0FBAC2-90D7-4FE3-825E-A2D4C439BF42}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>